<commit_message>
Version 1 de la app
</commit_message>
<xml_diff>
--- a/guestbook_entries.xlsx
+++ b/guestbook_entries.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,28 +468,56 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>asdas</t>
+          <t>Andrea Castillo</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>181485892</t>
+          <t>20985370-1</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>123123</t>
+          <t>21</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>12312</t>
+          <t>986389894</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2023-11-23 23:55:22</t>
+          <t>2023-11-24 10:58:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Sofia Martinez</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>11161499-7</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>934393434</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>2023-11-24 10:58:31</t>
         </is>
       </c>
     </row>

</xml_diff>